<commit_message>
GetEmails and CallWorkflow for specific BP
Signed-off-by: v-hansdavin <v-hans.davin@traveloka.com>
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HansDavinChristian\#Hans\Projects\Traveloka\UiPath\Sprint 2\Traveloka_DataAutomation_Performer_Email_S2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C033B9-D367-4C94-B7CA-4945F1ACEC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BEA070-32D1-4783-A2D8-F62D9B1B0EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -183,9 +183,6 @@
     <t>EmailRawFolderName</t>
   </si>
   <si>
-    <t>RPA_Moon_Cred_Gmail</t>
-  </si>
-  <si>
     <t>[Dev] RPA_Moon_UploadBucket</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>[Dev] RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_Cred_Gmail</t>
   </si>
 </sst>
 </file>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -656,7 +656,7 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -664,7 +664,7 @@
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -672,7 +672,7 @@
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -680,7 +680,7 @@
         <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2846,7 +2846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2899,7 +2899,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Change variable name, convert xls to xlsx using powershell, get converter path from asset
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HansDavinChristian\#Hans\Projects\Traveloka\UiPath\Sprint 2\Traveloka_DataAutomation_Performer_Email_S2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hans Davin\#Work\PT. Kalyana Adikarya Abadi\Projects\Traveloka\UiPath\Sprint 2\Traveloka_DataAutomation_Performer_Email_S2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BEA070-32D1-4783-A2D8-F62D9B1B0EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B556DF9-330D-44FA-844D-19FA5E3C0109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>[Dev] RPA_Moon_Cred_Gmail</t>
+  </si>
+  <si>
+    <t>ConverterPath</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathExcel</t>
   </si>
 </sst>
 </file>
@@ -573,16 +579,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -630,7 +636,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -640,7 +646,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1687,12 +1693,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1729,7 +1735,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1740,7 +1746,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1854,7 +1860,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2846,16 +2852,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2910,7 +2916,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add_Queue_Retry, SetTransStatus, Config.xlsx new asset
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hans Davin\#Work\PT. Kalyana Adikarya Abadi\Projects\Traveloka\UiPath\Sprint 2\Traveloka_DataAutomation_Performer_Email_S2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HansDavinChristian\#Hans\Projects\Traveloka\UiPath\Sprint 2\Traveloka_DataAutomation_Performer_Email_S2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B556DF9-330D-44FA-844D-19FA5E3C0109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6767B9-1B97-42E7-B80C-2E7089B6953D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -202,6 +202,18 @@
   </si>
   <si>
     <t>RPA_Moon_PathExcel</t>
+  </si>
+  <si>
+    <t>RPA_Moon_AutoRetryMax</t>
+  </si>
+  <si>
+    <t>AutoRetryMax</t>
+  </si>
+  <si>
+    <t>RPA_Moon_AutoRetryPostpone</t>
+  </si>
+  <si>
+    <t>AutoRetryPostpone</t>
   </si>
 </sst>
 </file>
@@ -583,12 +595,12 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -636,7 +648,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -646,7 +658,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1693,12 +1705,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1735,7 +1747,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1746,7 +1758,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1860,7 +1872,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2853,15 +2865,15 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2924,8 +2936,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added [Dev] to RPA_Moon_PathExcel (xls converter)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HansDavinChristian\#Hans\Projects\Traveloka\UiPath\Sprint 2\Traveloka_DataAutomation_Performer_Email_S2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6767B9-1B97-42E7-B80C-2E7089B6953D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86339904-8017-456A-BBAD-D6DE560EA19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,9 +201,6 @@
     <t>ConverterPath</t>
   </si>
   <si>
-    <t>RPA_Moon_PathExcel</t>
-  </si>
-  <si>
     <t>RPA_Moon_AutoRetryMax</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>AutoRetryPostpone</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathExcel</t>
   </si>
 </sst>
 </file>
@@ -2865,7 +2865,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2933,23 +2933,23 @@
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Removed attachment validation for Mickey
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 2\Traveloka_DataAutomation_Performer_Email_S2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D56AAD-E65D-47E2-9135-F17B38554107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71400438-EAF0-4260-87FB-A0BCC4BC481C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -213,9 +213,6 @@
     <t>[Dev] RPA_Moon_PathExcel</t>
   </si>
   <si>
-    <t>RPA_Moon_Cred_Gmail</t>
-  </si>
-  <si>
     <t>AutoRetryMaxDay</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>AutoRetrySchedule</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_Cred_Gmail</t>
   </si>
 </sst>
 </file>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -686,7 +686,7 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -2876,7 +2876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -2966,18 +2966,18 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
         <v>63</v>
-      </c>
-      <c r="B7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>